<commit_message>
mapping of district in gdansk updated for real-life purposes
</commit_message>
<xml_diff>
--- a/project/data_prepocessing/data_preprocesing_idea.xlsx
+++ b/project/data_prepocessing/data_preprocesing_idea.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusz/Documents/Code/masters_thesis/project/data_prepocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F905CBD0-9EB4-C94C-BDC0-A8617AD346D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A41A06-DD41-7649-A02F-B7272E51309E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34540" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{8BFF93E3-0FEE-C14C-97E3-AF563232A34E}"/>
+    <workbookView xWindow="7480" yWindow="3920" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{8BFF93E3-0FEE-C14C-97E3-AF563232A34E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="columns" sheetId="1" r:id="rId1"/>
+    <sheet name="districts_gda" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
   <si>
     <t>Trojmiasto</t>
   </si>
@@ -225,13 +226,142 @@
   </si>
   <si>
     <t>typ ogrzewnia</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Globalna</t>
+  </si>
+  <si>
+    <t>Srodmiescie</t>
+  </si>
+  <si>
+    <t>Przymorze wielkie</t>
+  </si>
+  <si>
+    <t>Przymorze male</t>
+  </si>
+  <si>
+    <t>Brzezno</t>
+  </si>
+  <si>
+    <t>Wrzeszcz</t>
+  </si>
+  <si>
+    <t>Zabianka - Wejhera - Jelitkowo - Tysiaclecia</t>
+  </si>
+  <si>
+    <t>Chełm z Południe</t>
+  </si>
+  <si>
+    <t>Jasień</t>
+  </si>
+  <si>
+    <t>Ujeścisko Łostowice</t>
+  </si>
+  <si>
+    <t>Letnica</t>
+  </si>
+  <si>
+    <t>Piecki - Migowo</t>
+  </si>
+  <si>
+    <t>Zaspa Młyniec</t>
+  </si>
+  <si>
+    <t>Orunia - Św. Wojciech - Lipce</t>
+  </si>
+  <si>
+    <t>Zaspa Rozstaje</t>
+  </si>
+  <si>
+    <t>Siedlce</t>
+  </si>
+  <si>
+    <t>Stogi z Przeróbką</t>
+  </si>
+  <si>
+    <t>Oliwa</t>
+  </si>
+  <si>
+    <t>Aniołki</t>
+  </si>
+  <si>
+    <t>Mickiewicza</t>
+  </si>
+  <si>
+    <t>Matarnia</t>
+  </si>
+  <si>
+    <t>Suchanino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brętowo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kokoszki </t>
+  </si>
+  <si>
+    <t>Strzyża</t>
+  </si>
+  <si>
+    <t>Młyniska</t>
+  </si>
+  <si>
+    <t>Jelitkowo</t>
+  </si>
+  <si>
+    <t>Chełm</t>
+  </si>
+  <si>
+    <t>Kokoszki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letnica </t>
+  </si>
+  <si>
+    <t>Nowy Port</t>
+  </si>
+  <si>
+    <t>Olszynka</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Orunia Górna - Gdańsk Południe</t>
+  </si>
+  <si>
+    <t>Osowa</t>
+  </si>
+  <si>
+    <t>Przeróbka</t>
+  </si>
+  <si>
+    <t>Stogi</t>
+  </si>
+  <si>
+    <t>Tysiąclecia</t>
+  </si>
+  <si>
+    <t>VII Dwór</t>
+  </si>
+  <si>
+    <t>Wejhera</t>
+  </si>
+  <si>
+    <t>Wrzeszc Dolny</t>
+  </si>
+  <si>
+    <t>Wrzeszc Górny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -257,6 +387,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
     </font>
   </fonts>
   <fills count="6">
@@ -303,18 +438,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,11 +765,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607AC7D4-A941-4A44-BD7C-990B7B15AD0F}">
   <dimension ref="B1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
@@ -648,7 +782,7 @@
     <col min="12" max="12" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:15">
       <c r="B1" t="s">
         <v>30</v>
       </c>
@@ -674,359 +808,323 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15">
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="8" spans="2:15">
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+    <row r="9" spans="2:15">
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="E10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="7" t="s">
+    <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
         <v>37</v>
       </c>
+      <c r="L10" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>22</v>
+    <row r="11" spans="2:15">
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>19</v>
+    <row r="12" spans="2:15">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="K12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15">
       <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="4"/>
+    <row r="15" spans="2:15">
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+    <row r="16" spans="2:15">
       <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+    <row r="17" spans="2:18">
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:18">
       <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:18">
       <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>14</v>
+        <v>59</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>24</v>
-      </c>
+    <row r="20" spans="2:18">
       <c r="E20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>24</v>
       </c>
       <c r="O20" s="2"/>
@@ -1034,130 +1132,146 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>24</v>
-      </c>
+    <row r="21" spans="2:18">
       <c r="O21" s="2"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:18">
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
       <c r="O22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H23" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" t="s">
-        <v>41</v>
-      </c>
+    <row r="23" spans="2:18">
       <c r="O23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:18">
+      <c r="H24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" t="s">
+        <v>46</v>
+      </c>
       <c r="O24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:18">
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H25" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="O25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:18">
       <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>15</v>
+        <v>62</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="O26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:18">
       <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="O27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:18">
       <c r="H28" t="s">
         <v>48</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="6" t="s">
         <v>20</v>
       </c>
       <c r="O28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="C29" s="4"/>
+    <row r="29" spans="2:18">
+      <c r="C29" s="2"/>
       <c r="H29" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K29" t="s">
         <v>38</v>
       </c>
-      <c r="L29" s="8" t="s">
+      <c r="L29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="O29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:18">
       <c r="E30" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>25</v>
       </c>
       <c r="O30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:18">
       <c r="E31" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:18">
       <c r="E32" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="6" t="s">
         <v>27</v>
       </c>
       <c r="M32" s="1" t="s">
@@ -1166,11 +1280,11 @@
       <c r="O32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:18">
       <c r="E33" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H33" t="s">
@@ -1183,72 +1297,596 @@
       <c r="O33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:18">
       <c r="M34" s="2"/>
       <c r="O34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:18">
       <c r="M35" s="2"/>
       <c r="O35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C36" s="2"/>
+    <row r="36" spans="5:18">
       <c r="M36" s="2"/>
       <c r="O36" s="2"/>
       <c r="R36" s="2"/>
     </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:18">
       <c r="M37" s="2"/>
       <c r="O37" s="2"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:18">
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:18">
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:18">
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:18">
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:18">
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:18">
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:18">
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:18">
       <c r="M45" s="2"/>
     </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:18">
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:18">
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:18">
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="13:13">
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="13:13">
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="13:13">
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="13:13">
       <c r="M52" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45324EAF-50AC-214D-B8D4-5AF0FA3EC05C}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="37.5" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="C2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="E6" s="9"/>
+      <c r="F6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6">
+        <v>43</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="E7" s="9"/>
+      <c r="F7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7">
+        <v>32</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="E8" s="9"/>
+      <c r="F8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8">
+        <v>33</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="E9" s="9"/>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="E10" s="9"/>
+      <c r="I10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="E11" s="9"/>
+      <c r="I11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="E12" s="9"/>
+      <c r="I12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="E13" s="9"/>
+      <c r="I13" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="E14" s="9"/>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="E15" s="9"/>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="E16" s="9"/>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10">
+      <c r="E17" s="9"/>
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10">
+      <c r="E18" s="9"/>
+      <c r="F18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18">
+        <v>14</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10">
+      <c r="E19" s="9"/>
+      <c r="F19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19">
+        <v>14</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10">
+      <c r="E20" s="9"/>
+      <c r="F20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10">
+      <c r="E21" s="9"/>
+      <c r="F21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10">
+      <c r="E22" s="9"/>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10">
+      <c r="E23" s="9"/>
+      <c r="I23" t="s">
+        <v>97</v>
+      </c>
+      <c r="J23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10">
+      <c r="E24" s="9"/>
+      <c r="F24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24">
+        <v>9</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10">
+      <c r="E25" s="9"/>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10">
+      <c r="E26" s="9"/>
+      <c r="F26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26">
+        <v>7</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10">
+      <c r="E27" s="9"/>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10">
+      <c r="E28" s="9"/>
+      <c r="F28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10">
+      <c r="E29" s="9"/>
+      <c r="F29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10">
+      <c r="E30" s="9"/>
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>84</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10">
+      <c r="E31" s="9"/>
+      <c r="F31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10">
+      <c r="E32" s="9"/>
+      <c r="F32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10">
+      <c r="E33" s="9"/>
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10">
+      <c r="E34" s="9"/>
+      <c r="F34" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10">
+      <c r="E35" s="9"/>
+      <c r="F35" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10">
+      <c r="F36" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="5:10">
+      <c r="I37" t="s">
+        <v>95</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="5:10">
+      <c r="I38" t="s">
+        <v>96</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="5:10">
+      <c r="I39" t="s">
+        <v>98</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="5:10">
+      <c r="I40" t="s">
+        <v>99</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="5:10">
+      <c r="I41" t="s">
+        <v>100</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="5:10">
+      <c r="I42" t="s">
+        <v>86</v>
+      </c>
+      <c r="J42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="5:10">
+      <c r="I43" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
locations changed properly for olx
</commit_message>
<xml_diff>
--- a/project/data_prepocessing/data_preprocesing_idea.xlsx
+++ b/project/data_prepocessing/data_preprocesing_idea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusz/Documents/Code/masters_thesis/project/data_prepocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A41A06-DD41-7649-A02F-B7272E51309E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9D3970-7007-A24D-A57B-1EE2CEFBC96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7480" yWindow="3920" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{8BFF93E3-0FEE-C14C-97E3-AF563232A34E}"/>
+    <workbookView xWindow="1020" yWindow="1460" windowWidth="28040" windowHeight="17440" xr2:uid="{8BFF93E3-0FEE-C14C-97E3-AF563232A34E}"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="184">
   <si>
     <t>Trojmiasto</t>
   </si>
@@ -234,9 +234,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>Globalna</t>
-  </si>
-  <si>
     <t>Srodmiescie</t>
   </si>
   <si>
@@ -300,9 +297,6 @@
     <t>Suchanino</t>
   </si>
   <si>
-    <t xml:space="preserve">Brętowo </t>
-  </si>
-  <si>
     <t xml:space="preserve">Kokoszki </t>
   </si>
   <si>
@@ -355,6 +349,246 @@
   </si>
   <si>
     <t>Wrzeszc Górny</t>
+  </si>
+  <si>
+    <t>Śródmieście</t>
+  </si>
+  <si>
+    <t>Żabianka</t>
+  </si>
+  <si>
+    <t>Brętowo</t>
+  </si>
+  <si>
+    <t>Gdansk</t>
+  </si>
+  <si>
+    <t>Przymorze</t>
+  </si>
+  <si>
+    <t>pomorskie</t>
+  </si>
+  <si>
+    <t>Stare Miasto</t>
+  </si>
+  <si>
+    <t>Brzeźno</t>
+  </si>
+  <si>
+    <t>Zaspa-Rozstaje</t>
+  </si>
+  <si>
+    <t>Zaspa</t>
+  </si>
+  <si>
+    <t>Piecki-Migowo</t>
+  </si>
+  <si>
+    <t>Ujeścisko</t>
+  </si>
+  <si>
+    <t>Łostowice</t>
+  </si>
+  <si>
+    <t>Dolne Miasto</t>
+  </si>
+  <si>
+    <t>Główne Miato</t>
+  </si>
+  <si>
+    <t>Stare Przedmieście</t>
+  </si>
+  <si>
+    <t>Wrzeszcz Dolny</t>
+  </si>
+  <si>
+    <t>Przymorze Wielkie</t>
+  </si>
+  <si>
+    <t>Orunia</t>
+  </si>
+  <si>
+    <t>Maćkowy</t>
+  </si>
+  <si>
+    <t>Kiełpinek</t>
+  </si>
+  <si>
+    <t>Długie Gorody</t>
+  </si>
+  <si>
+    <t>Morena</t>
+  </si>
+  <si>
+    <t>Dolne</t>
+  </si>
+  <si>
+    <t>Zakoniczyn</t>
+  </si>
+  <si>
+    <t>Stare</t>
+  </si>
+  <si>
+    <t>Długie</t>
+  </si>
+  <si>
+    <t>Kowale:</t>
+  </si>
+  <si>
+    <t>Nowy:</t>
+  </si>
+  <si>
+    <t>Oliwa:</t>
+  </si>
+  <si>
+    <t>Ujeścisko:</t>
+  </si>
+  <si>
+    <t>Piecki:</t>
+  </si>
+  <si>
+    <t>Jelitkowo:</t>
+  </si>
+  <si>
+    <t>Jelitkowski:</t>
+  </si>
+  <si>
+    <t>Południe:</t>
+  </si>
+  <si>
+    <t>Siedle:</t>
+  </si>
+  <si>
+    <t>Osowa:</t>
+  </si>
+  <si>
+    <t>Antoniego:</t>
+  </si>
+  <si>
+    <t>Przeróbka:</t>
+  </si>
+  <si>
+    <t>Chełm:</t>
+  </si>
+  <si>
+    <t>Osiedle:</t>
+  </si>
+  <si>
+    <t>Młode:</t>
+  </si>
+  <si>
+    <t>Podwale:</t>
+  </si>
+  <si>
+    <t>Czarny:</t>
+  </si>
+  <si>
+    <t>Długie:</t>
+  </si>
+  <si>
+    <t>Piecki-:</t>
+  </si>
+  <si>
+    <t>Maćkowy:</t>
+  </si>
+  <si>
+    <t>G:</t>
+  </si>
+  <si>
+    <t>Łostwice:</t>
+  </si>
+  <si>
+    <t>Kiełpinek:</t>
+  </si>
+  <si>
+    <t>V:</t>
+  </si>
+  <si>
+    <t>Nowa:</t>
+  </si>
+  <si>
+    <t>Angielska:</t>
+  </si>
+  <si>
+    <t>Letnica37:</t>
+  </si>
+  <si>
+    <t>Karczemki:</t>
+  </si>
+  <si>
+    <t>Cygańska:</t>
+  </si>
+  <si>
+    <t>Ofiar:</t>
+  </si>
+  <si>
+    <t>Bora-:</t>
+  </si>
+  <si>
+    <t>Starówka:</t>
+  </si>
+  <si>
+    <t>Przymorzeul.:</t>
+  </si>
+  <si>
+    <t>Garnizon:</t>
+  </si>
+  <si>
+    <t>Przymorze10:</t>
+  </si>
+  <si>
+    <t>Sródmieście</t>
+  </si>
+  <si>
+    <t>Obrońców</t>
+  </si>
+  <si>
+    <t>Wzgórze</t>
+  </si>
+  <si>
+    <t>Ul</t>
+  </si>
+  <si>
+    <t>Rebiechowo</t>
+  </si>
+  <si>
+    <t>Suchaninovan</t>
+  </si>
+  <si>
+    <t>Morenagen</t>
+  </si>
+  <si>
+    <t>GLOBALNA</t>
+  </si>
+  <si>
+    <t>Zabianka-Wejhera-Jelitkowo-Tysiaclecia</t>
+  </si>
+  <si>
+    <t>will be</t>
+  </si>
+  <si>
+    <t>Chełm - Łostowice - Południe - Orunia</t>
+  </si>
+  <si>
+    <t>Piecki-Migowo - Suchanino - Morena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matarnia - Kokoszki </t>
+  </si>
+  <si>
+    <t>Brzeźno - Nowy Port</t>
+  </si>
+  <si>
+    <t>Oliwa - Strzyża</t>
+  </si>
+  <si>
+    <t>Przeróbka - Stogi</t>
+  </si>
+  <si>
+    <t>Siedlce - Aniołki - Młyniska</t>
+  </si>
+  <si>
+    <t>Śródmieście - Stare Miasto - Dolne Miasto - Długie Ogrody</t>
   </si>
 </sst>
 </file>
@@ -394,7 +628,7 @@
       <name val="Var(--jp-code-font-family)"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +659,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -438,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -448,7 +688,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607AC7D4-A941-4A44-BD7C-990B7B15AD0F}">
   <dimension ref="B1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:L1"/>
     </sheetView>
   </sheetViews>
@@ -1371,525 +1618,1317 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45324EAF-50AC-214D-B8D4-5AF0FA3EC05C}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="C1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="37.5" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="37.5" customWidth="1"/>
+    <col min="9" max="9" width="38.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="12"/>
+    <col min="11" max="11" width="29.6640625" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" customWidth="1"/>
+    <col min="13" max="13" width="40.83203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="12"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="17" max="17" width="38.1640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="4"/>
+    <row r="1" spans="1:23">
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="14"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="4"/>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="W1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="D2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="K4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L4">
+        <v>142</v>
+      </c>
+      <c r="O4" t="s">
+        <v>109</v>
+      </c>
+      <c r="P4">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>110</v>
+      </c>
+      <c r="S4">
+        <v>15</v>
+      </c>
+      <c r="V4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5">
+        <v>78</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5">
+        <v>218</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O5" t="s">
+        <v>104</v>
+      </c>
+      <c r="P5">
+        <v>83</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="R5" t="s">
+        <v>117</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="V5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6">
+        <v>43</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6">
+        <v>58</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O6" t="s">
+        <v>121</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" t="s">
+        <v>118</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="V6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7">
+        <v>32</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7">
+        <v>56</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="R7" t="s">
+        <v>119</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="V7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8">
+        <v>33</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8">
+        <v>46</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="O8" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R8" t="s">
+        <v>125</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="V8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9">
+        <v>32</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9">
+        <v>38</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" t="s">
+        <v>120</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10">
+        <v>38</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="C2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="E6" s="9"/>
-      <c r="F6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6">
-        <v>43</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="E7" s="9"/>
-      <c r="F7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7">
-        <v>32</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="E8" s="9"/>
-      <c r="F8" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G8">
-        <v>33</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="E9" s="9"/>
-      <c r="F9" t="s">
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="V10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="E10" s="9"/>
-      <c r="I10" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="E11" s="9"/>
+      <c r="H11">
+        <v>30</v>
+      </c>
       <c r="I11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J11">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="E12" s="9"/>
+      <c r="L11">
+        <v>14</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O11" t="s">
+        <v>105</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="I12" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12">
+        <v>174</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="E13" s="9"/>
-      <c r="I13" t="s">
-        <v>101</v>
-      </c>
-      <c r="J13">
+      <c r="M12" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="E14" s="9"/>
-      <c r="I14" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14">
+      <c r="M13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="E15" s="9"/>
-      <c r="F15" t="s">
+      <c r="M14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O14" t="s">
+        <v>89</v>
+      </c>
+      <c r="P14">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="B15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="E16" s="9"/>
-      <c r="I16" t="s">
-        <v>92</v>
-      </c>
-      <c r="J16">
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="L15">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="9"/>
-      <c r="F17" t="s">
+      <c r="M15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="O15" t="s">
+        <v>90</v>
+      </c>
+      <c r="P15">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="V15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="C16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16">
+        <v>23</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="O16" t="s">
+        <v>122</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="V16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="D17" t="s">
         <v>72</v>
       </c>
-      <c r="G17">
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17">
+        <v>24</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O17" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="5:10">
-      <c r="E18" s="9"/>
-      <c r="F18" s="3" t="s">
+      <c r="Q17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="V17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>14</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J18">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10">
-      <c r="E19" s="9"/>
-      <c r="F19" s="3" t="s">
+      <c r="L18">
+        <v>15</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="O18" t="s">
+        <v>115</v>
+      </c>
+      <c r="P18">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="R18">
+        <v>5</v>
+      </c>
+      <c r="V18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="G19">
-        <v>14</v>
+      <c r="F19" s="13"/>
+      <c r="G19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J19">
+      <c r="K19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19">
+        <v>18</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="V19" s="10"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="C20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20">
+        <v>16</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="O20" t="s">
+        <v>114</v>
+      </c>
+      <c r="P20">
+        <v>7</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="F21" s="13"/>
+      <c r="G21" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21">
+        <v>12</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" t="s">
+        <v>113</v>
+      </c>
+      <c r="P21">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22">
+        <v>17</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="O22" t="s">
+        <v>112</v>
+      </c>
+      <c r="P22">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" t="s">
+        <v>97</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O24" t="s">
+        <v>97</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="E25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L26">
+        <v>12</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="O26" t="s">
+        <v>79</v>
+      </c>
+      <c r="P26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="D27" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27">
+        <v>24</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="O27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P27">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="5:10">
-      <c r="E20" s="9"/>
-      <c r="F20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20">
-        <v>12</v>
-      </c>
-      <c r="I20" s="3" t="s">
+      <c r="Q27" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="F28" s="13"/>
+      <c r="G28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="D29" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="C30" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+      <c r="O31" t="s">
+        <v>85</v>
+      </c>
+      <c r="P31">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="B32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32" t="s">
+        <v>178</v>
+      </c>
+      <c r="O32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17">
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17">
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="L34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17">
+      <c r="C35" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="3:17">
+      <c r="G36" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17">
+      <c r="D37" t="s">
+        <v>132</v>
+      </c>
+      <c r="K37" t="s">
+        <v>93</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="O37" t="s">
+        <v>93</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="3:17">
+      <c r="K38" t="s">
         <v>94</v>
       </c>
-      <c r="J20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="5:10">
-      <c r="E21" s="9"/>
-      <c r="F21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21">
-        <v>10</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J21">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="5:10">
-      <c r="E22" s="9"/>
-      <c r="F22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22">
-        <v>10</v>
-      </c>
-      <c r="I22" t="s">
-        <v>77</v>
-      </c>
-      <c r="J22">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10">
-      <c r="E23" s="9"/>
-      <c r="I23" t="s">
-        <v>97</v>
-      </c>
-      <c r="J23">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="5:10">
-      <c r="E24" s="9"/>
-      <c r="F24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24">
-        <v>9</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24">
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="O38" t="s">
+        <v>96</v>
+      </c>
+      <c r="P38">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="3:17">
+      <c r="D39" t="s">
+        <v>140</v>
+      </c>
+      <c r="K39" t="s">
+        <v>96</v>
+      </c>
+      <c r="L39">
+        <v>3</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="3:17">
+      <c r="K41" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="5:10">
-      <c r="E25" s="9"/>
-      <c r="F25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="5:10">
-      <c r="E26" s="9"/>
-      <c r="F26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26">
-        <v>7</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="5:10">
-      <c r="E27" s="9"/>
-      <c r="F27" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="5:10">
-      <c r="E28" s="9"/>
-      <c r="F28" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G28">
-        <v>5</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J28">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="5:10">
-      <c r="E29" s="9"/>
-      <c r="F29" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29">
-        <v>5</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J29">
+    <row r="42" spans="3:17">
+      <c r="C42" t="s">
+        <v>150</v>
+      </c>
+      <c r="O42" t="s">
+        <v>123</v>
+      </c>
+      <c r="P42">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="5:10">
-      <c r="E30" s="9"/>
-      <c r="F30" t="s">
-        <v>84</v>
-      </c>
-      <c r="G30">
+    <row r="43" spans="3:17">
+      <c r="O43" t="s">
+        <v>124</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="3:17">
+      <c r="O44" t="s">
+        <v>98</v>
+      </c>
+      <c r="P44">
         <v>2</v>
       </c>
-      <c r="I30" t="s">
-        <v>84</v>
-      </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="5:10">
-      <c r="E31" s="9"/>
-      <c r="F31" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10">
-      <c r="E32" s="9"/>
-      <c r="F32" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32">
-        <v>2</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10">
-      <c r="E33" s="9"/>
-      <c r="F33" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="5:10">
-      <c r="E34" s="9"/>
-      <c r="F34" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="J34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="5:10">
-      <c r="E35" s="9"/>
-      <c r="F35" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="5:10">
-      <c r="F36" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="5:10">
-      <c r="I37" t="s">
-        <v>95</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="5:10">
-      <c r="I38" t="s">
-        <v>96</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="5:10">
-      <c r="I39" t="s">
-        <v>98</v>
-      </c>
-      <c r="J39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="5:10">
-      <c r="I40" t="s">
-        <v>99</v>
-      </c>
-      <c r="J40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="5:10">
-      <c r="I41" t="s">
-        <v>100</v>
-      </c>
-      <c r="J41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="5:10">
-      <c r="I42" t="s">
-        <v>86</v>
-      </c>
-      <c r="J42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="5:10">
-      <c r="I43" t="s">
-        <v>102</v>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new data being processed
</commit_message>
<xml_diff>
--- a/project/data_prepocessing/data_preprocesing_idea.xlsx
+++ b/project/data_prepocessing/data_preprocesing_idea.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusz/Documents/Code/masters_thesis/project/data_prepocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9D3970-7007-A24D-A57B-1EE2CEFBC96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F603CA7B-28E7-634F-90AC-D175E97AF9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1460" windowWidth="28040" windowHeight="17440" xr2:uid="{8BFF93E3-0FEE-C14C-97E3-AF563232A34E}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="18740" xr2:uid="{8BFF93E3-0FEE-C14C-97E3-AF563232A34E}"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
     <sheet name="districts_gda" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -678,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -688,7 +688,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1013,7 +1012,7 @@
   <dimension ref="B1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1629,14 +1628,14 @@
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="11" customWidth="1"/>
     <col min="7" max="7" width="37.5" customWidth="1"/>
     <col min="9" max="9" width="38.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="12"/>
+    <col min="10" max="10" width="10.83203125" style="11"/>
     <col min="11" max="11" width="29.6640625" customWidth="1"/>
     <col min="12" max="12" width="19.83203125" customWidth="1"/>
     <col min="13" max="13" width="40.83203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="12"/>
+    <col min="14" max="14" width="10.83203125" style="11"/>
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="17" max="17" width="38.1640625" style="3" customWidth="1"/>
     <col min="22" max="22" width="18.1640625" customWidth="1"/>
@@ -1646,20 +1645,20 @@
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="11"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="11"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="10"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="11"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="10"/>
       <c r="O1" s="4"/>
       <c r="P1" t="s">
         <v>12</v>
@@ -1672,7 +1671,7 @@
       <c r="D2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>175</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1681,7 +1680,7 @@
       <c r="H2" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>175</v>
       </c>
       <c r="K2" s="4" t="s">
@@ -1707,7 +1706,7 @@
       <c r="A4" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="12"/>
       <c r="K4" t="s">
         <v>107</v>
       </c>
@@ -1743,7 +1742,7 @@
       <c r="E5" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="12"/>
       <c r="G5" t="s">
         <v>65</v>
       </c>
@@ -1788,8 +1787,8 @@
       <c r="E6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" t="s">
         <v>66</v>
       </c>
       <c r="H6">
@@ -1798,7 +1797,7 @@
       <c r="I6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" t="s">
         <v>66</v>
       </c>
       <c r="L6">
@@ -1842,8 +1841,8 @@
       <c r="E7" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" t="s">
         <v>67</v>
       </c>
       <c r="H7">
@@ -1852,7 +1851,7 @@
       <c r="I7" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" t="s">
         <v>67</v>
       </c>
       <c r="L7">
@@ -1884,14 +1883,14 @@
       <c r="A8" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="12"/>
+      <c r="G8" t="s">
         <v>68</v>
       </c>
       <c r="H8">
@@ -1900,7 +1899,7 @@
       <c r="I8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" t="s">
         <v>68</v>
       </c>
       <c r="L8">
@@ -1944,8 +1943,8 @@
       <c r="E9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" t="s">
         <v>69</v>
       </c>
       <c r="H9">
@@ -1954,7 +1953,7 @@
       <c r="I9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" t="s">
         <v>102</v>
       </c>
       <c r="L9">
@@ -1980,14 +1979,14 @@
       <c r="A10" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" t="s">
         <v>69</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" t="s">
         <v>103</v>
       </c>
       <c r="L10">
@@ -2022,8 +2021,8 @@
       <c r="E11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" t="s">
         <v>70</v>
       </c>
       <c r="H11">
@@ -2032,7 +2031,7 @@
       <c r="I11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" t="s">
         <v>105</v>
       </c>
       <c r="L11">
@@ -2064,14 +2063,14 @@
       <c r="E12" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="12"/>
+      <c r="G12" t="s">
         <v>70</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" t="s">
         <v>101</v>
       </c>
       <c r="L12">
@@ -2094,14 +2093,14 @@
       <c r="E13" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" t="s">
         <v>70</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" t="s">
         <v>99</v>
       </c>
       <c r="L13">
@@ -2124,14 +2123,14 @@
       <c r="E14" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="9" t="s">
+      <c r="F14" s="12"/>
+      <c r="G14" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" t="s">
         <v>89</v>
       </c>
       <c r="L14">
@@ -2163,23 +2162,23 @@
       <c r="D15" t="s">
         <v>143</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" t="s">
         <v>71</v>
       </c>
       <c r="H15">
         <v>17</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" t="s">
         <v>90</v>
       </c>
       <c r="L15">
         <v>11</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O15" t="s">
@@ -2188,7 +2187,7 @@
       <c r="P15">
         <v>4</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="13" t="s">
         <v>176</v>
       </c>
       <c r="V15" t="s">
@@ -2202,20 +2201,20 @@
       <c r="D16" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="9" t="s">
+      <c r="F16" s="12"/>
+      <c r="G16" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" t="s">
         <v>95</v>
       </c>
       <c r="L16">
         <v>23</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O16" t="s">
@@ -2224,7 +2223,7 @@
       <c r="P16">
         <v>2</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="Q16" s="13" t="s">
         <v>176</v>
       </c>
       <c r="V16" t="s">
@@ -2238,8 +2237,8 @@
       <c r="E17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="9" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" t="s">
         <v>72</v>
       </c>
       <c r="H17">
@@ -2248,7 +2247,7 @@
       <c r="I17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" t="s">
         <v>72</v>
       </c>
       <c r="L17">
@@ -2283,23 +2282,23 @@
       <c r="D18" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="9" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" t="s">
         <v>73</v>
       </c>
       <c r="H18">
         <v>14</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="K18" t="s">
         <v>73</v>
       </c>
       <c r="L18">
         <v>15</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O18" t="s">
@@ -2308,7 +2307,7 @@
       <c r="P18">
         <v>5</v>
       </c>
-      <c r="Q18" s="14" t="s">
+      <c r="Q18" s="13" t="s">
         <v>176</v>
       </c>
       <c r="R18">
@@ -2325,8 +2324,8 @@
       <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="9" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" t="s">
         <v>74</v>
       </c>
       <c r="H19">
@@ -2335,7 +2334,7 @@
       <c r="I19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="K19" t="s">
         <v>92</v>
       </c>
       <c r="L19">
@@ -2353,7 +2352,7 @@
       <c r="Q19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="V19" s="10"/>
+      <c r="V19" s="9"/>
     </row>
     <row r="20" spans="1:22">
       <c r="C20" t="s">
@@ -2362,8 +2361,8 @@
       <c r="D20" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="9" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" t="s">
         <v>75</v>
       </c>
       <c r="H20">
@@ -2372,7 +2371,7 @@
       <c r="I20" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" t="s">
         <v>75</v>
       </c>
       <c r="L20">
@@ -2395,8 +2394,8 @@
       </c>
     </row>
     <row r="21" spans="1:22">
-      <c r="F21" s="13"/>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" t="s">
         <v>76</v>
       </c>
       <c r="H21">
@@ -2405,7 +2404,7 @@
       <c r="I21" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" t="s">
         <v>76</v>
       </c>
       <c r="L21">
@@ -2428,8 +2427,8 @@
       <c r="C22" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="9" t="s">
+      <c r="F22" s="12"/>
+      <c r="G22" t="s">
         <v>78</v>
       </c>
       <c r="H22">
@@ -2438,7 +2437,7 @@
       <c r="I22" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" t="s">
         <v>78</v>
       </c>
       <c r="L22">
@@ -2461,23 +2460,23 @@
       <c r="A23" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="9" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" t="s">
         <v>77</v>
       </c>
       <c r="H23">
         <v>9</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="K23" t="s">
         <v>77</v>
       </c>
       <c r="L23">
         <v>4</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="13" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2491,8 +2490,8 @@
       <c r="E24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="9" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" t="s">
         <v>80</v>
       </c>
       <c r="H24">
@@ -2524,8 +2523,8 @@
       <c r="E25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="9" t="s">
+      <c r="F25" s="12"/>
+      <c r="G25" t="s">
         <v>80</v>
       </c>
       <c r="I25" s="3" t="s">
@@ -2551,14 +2550,14 @@
       <c r="E26" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="9" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" t="s">
         <v>79</v>
       </c>
       <c r="H26">
         <v>7</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="K26" t="s">
         <v>79</v>
       </c>
       <c r="L26">
@@ -2578,14 +2577,14 @@
       <c r="D27" t="s">
         <v>133</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="9" t="s">
+      <c r="F27" s="12"/>
+      <c r="G27" t="s">
         <v>81</v>
       </c>
       <c r="H27">
         <v>5</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="K27" t="s">
         <v>81</v>
       </c>
       <c r="L27">
@@ -2605,14 +2604,14 @@
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="F28" s="13"/>
-      <c r="G28" s="9" t="s">
+      <c r="F28" s="12"/>
+      <c r="G28" t="s">
         <v>82</v>
       </c>
       <c r="H28">
         <v>5</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" t="s">
         <v>82</v>
       </c>
       <c r="L28">
@@ -2626,8 +2625,8 @@
       <c r="E29" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="9" t="s">
+      <c r="F29" s="12"/>
+      <c r="G29" t="s">
         <v>83</v>
       </c>
       <c r="H29">
@@ -2636,7 +2635,7 @@
       <c r="I29" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" t="s">
         <v>83</v>
       </c>
       <c r="L29">
@@ -2656,8 +2655,8 @@
       <c r="E30" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="9" t="s">
+      <c r="F30" s="12"/>
+      <c r="G30" t="s">
         <v>84</v>
       </c>
       <c r="H30">
@@ -2666,7 +2665,7 @@
       <c r="I30" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" t="s">
         <v>84</v>
       </c>
       <c r="L30">
@@ -2686,14 +2685,14 @@
       <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="9" t="s">
+      <c r="F31" s="12"/>
+      <c r="G31" t="s">
         <v>85</v>
       </c>
       <c r="H31">
         <v>2</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="K31" t="s">
         <v>85</v>
       </c>
       <c r="L31">
@@ -2719,8 +2718,8 @@
       <c r="D32" t="s">
         <v>91</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="9" t="s">
+      <c r="F32" s="12"/>
+      <c r="G32" t="s">
         <v>86</v>
       </c>
       <c r="H32">
@@ -2729,7 +2728,7 @@
       <c r="I32" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="K32" t="s">
         <v>91</v>
       </c>
       <c r="L32">
@@ -2752,14 +2751,14 @@
       <c r="D33" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="9" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" t="s">
         <v>87</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="K33" t="s">
         <v>87</v>
       </c>
       <c r="L33">
@@ -2770,14 +2769,14 @@
       <c r="C34" t="s">
         <v>113</v>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="9" t="s">
+      <c r="F34" s="12"/>
+      <c r="G34" t="s">
         <v>88</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" t="s">
         <v>88</v>
       </c>
       <c r="L34">
@@ -2788,10 +2787,10 @@
       <c r="C35" t="s">
         <v>169</v>
       </c>
-      <c r="F35" s="13"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="3:17">
-      <c r="G36" s="9" t="s">
+      <c r="G36" t="s">
         <v>106</v>
       </c>
       <c r="H36">

</xml_diff>